<commit_message>
adding provider to ballon
</commit_message>
<xml_diff>
--- a/INVENTARIOS DEPOSITO/BALON 6-8-2022.xlsx
+++ b/INVENTARIOS DEPOSITO/BALON 6-8-2022.xlsx
@@ -408,16 +408,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X12" activeCellId="0" sqref="X12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z15" activeCellId="0" sqref="Z15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="33"/>
@@ -503,7 +503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>26</v>
       </c>
@@ -549,6 +549,9 @@
       <c r="W2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="X2" s="0" t="n">
+        <v>25998807</v>
+      </c>
       <c r="Y2" s="0" t="n">
         <v>5</v>
       </c>
@@ -556,7 +559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>38</v>
       </c>
@@ -602,6 +605,9 @@
       <c r="W3" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="X3" s="0" t="n">
+        <v>25998807</v>
+      </c>
       <c r="Y3" s="0" t="n">
         <v>5</v>
       </c>
@@ -609,7 +615,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>41</v>
       </c>
@@ -655,6 +661,9 @@
       <c r="W4" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="X4" s="0" t="n">
+        <v>25998807</v>
+      </c>
       <c r="Y4" s="0" t="n">
         <v>5</v>
       </c>
@@ -662,7 +671,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>44</v>
       </c>
@@ -708,6 +717,9 @@
       <c r="W5" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="X5" s="0" t="n">
+        <v>25998807</v>
+      </c>
       <c r="Y5" s="0" t="n">
         <v>5</v>
       </c>
@@ -715,7 +727,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>47</v>
       </c>
@@ -761,6 +773,9 @@
       <c r="W6" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="X6" s="0" t="n">
+        <v>25998807</v>
+      </c>
       <c r="Y6" s="0" t="n">
         <v>5</v>
       </c>
@@ -768,7 +783,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>50</v>
       </c>
@@ -814,6 +829,9 @@
       <c r="W7" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="X7" s="0" t="n">
+        <v>25998807</v>
+      </c>
       <c r="Y7" s="0" t="n">
         <v>5</v>
       </c>
@@ -821,7 +839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>53</v>
       </c>
@@ -867,6 +885,9 @@
       <c r="W8" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="X8" s="0" t="n">
+        <v>25998807</v>
+      </c>
       <c r="Y8" s="0" t="n">
         <v>5</v>
       </c>
@@ -874,7 +895,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>56</v>
       </c>
@@ -920,6 +941,9 @@
       <c r="W9" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="X9" s="0" t="n">
+        <v>25998807</v>
+      </c>
       <c r="Y9" s="0" t="n">
         <v>5</v>
       </c>
@@ -927,7 +951,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>59</v>
       </c>
@@ -973,6 +997,9 @@
       <c r="W10" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="X10" s="0" t="n">
+        <v>25998807</v>
+      </c>
       <c r="Y10" s="0" t="n">
         <v>5</v>
       </c>
@@ -980,6 +1007,7 @@
         <v>55</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>